<commit_message>
Add Week2 Day7 session management deep-dive analysis
- 완료: chat_session 생명주기 및 메모리 관리 심화 분석
- 핵심 개념: shared_from_this 패턴과 ref_count 메커니즘
- 각 비동기 작업이 자기 몫의 ref_count를 확보하여 안전성 보장
- io_context와 비동기 핸들러 큐의 동작 원리 이해
- session_management_analysis.md 작성 완료
- CLAUDE.md 업데이트 (Day7 완료 표시)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Pass1_게임서버_4주_학습계획.xlsx
+++ b/Pass1_게임서버_4주_학습계획.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Others\boost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC49C96C-72AC-4403-B4C7-E68CAE9EC6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4606104F-A943-422E-B2FA-6630AD8FDD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
   <si>
     <t>일차</t>
   </si>
@@ -354,13 +354,17 @@
   </si>
   <si>
     <t>핵심 패턴 정리, 문서화</t>
+  </si>
+  <si>
+    <t>☑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +386,12 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI Symbol"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -410,9 +420,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -718,7 +729,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -844,8 +855,8 @@
       <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" t="s">
-        <v>12</v>
+      <c r="G5" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -867,8 +878,8 @@
       <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="G6" t="s">
-        <v>28</v>
+      <c r="G6" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -890,8 +901,8 @@
       <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="G7" t="s">
-        <v>28</v>
+      <c r="G7" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add Week2 Day9 chat_client analysis
- 스레드 분리 패턴 분석 (메인: 입력, I/O: 송수신)
- post/dispatch/defer 작업 제출 방법 비교
- strand를 통한 핸들러 직렬화 패턴 학습

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Pass1_게임서버_4주_학습계획.xlsx
+++ b/Pass1_게임서버_4주_학습계획.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Others\boost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4606104F-A943-422E-B2FA-6630AD8FDD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1078A4EF-D6E6-41F5-B167-64BD99853DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -729,7 +729,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -924,8 +924,8 @@
       <c r="F8" t="s">
         <v>44</v>
       </c>
-      <c r="G8" t="s">
-        <v>28</v>
+      <c r="G8" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -947,8 +947,8 @@
       <c r="F9" t="s">
         <v>49</v>
       </c>
-      <c r="G9" t="s">
-        <v>28</v>
+      <c r="G9" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -1230,5 +1230,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>